<commit_message>
Updated data for O.punctata
</commit_message>
<xml_diff>
--- a/Data/Photosynthetic rates at the growth CO2.xlsx
+++ b/Data/Photosynthetic rates at the growth CO2.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://campusruacza-my.sharepoint.com/personal/g12f2166_campusruacza_onmicrosoft_com/Documents/M.Sc Project/M.Sc Project/Oxalis punctata 2017/ACi curves/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CO2-effects-on-geophytes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="671" documentId="13_ncr:1_{00FC013A-D6C9-41A8-B6F3-2E7D7D948ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F290F21-9F40-460A-88BD-6102698F1F6B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8A551C-A535-4425-AF22-1DFFA83B680D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="1000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stomatal limitation" sheetId="4" r:id="rId1"/>
     <sheet name="Photosynthetic rates" sheetId="3" r:id="rId2"/>
-    <sheet name="50% Long Ashton" sheetId="1" r:id="rId3"/>
-    <sheet name="100% Long Ashton" sheetId="2" r:id="rId4"/>
-    <sheet name="Curves plotted in R" sheetId="5" r:id="rId5"/>
+    <sheet name="Stomatalconductance" sheetId="6" r:id="rId3"/>
+    <sheet name="50% Long Ashton" sheetId="1" r:id="rId4"/>
+    <sheet name="100% Long Ashton" sheetId="2" r:id="rId5"/>
+    <sheet name="Curves plotted in R" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="37">
   <si>
     <t>CO2S</t>
   </si>
@@ -528,9 +529,9 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -541,7 +542,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>17.532971295577966</v>
       </c>
@@ -552,7 +553,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>22.117541498429787</v>
       </c>
@@ -563,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>18.156424581005581</v>
       </c>
@@ -574,7 +575,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>11.108490566037737</v>
       </c>
@@ -585,7 +586,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>13.581599123767793</v>
       </c>
@@ -596,7 +597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>13.809523809523814</v>
       </c>
@@ -607,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7.2747014115092172</v>
       </c>
@@ -618,7 +619,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7.7738515901060161</v>
       </c>
@@ -629,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>15.109235495076504</v>
       </c>
@@ -640,7 +641,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>16.158357771261002</v>
       </c>
@@ -651,7 +652,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>16.158357771261002</v>
       </c>
@@ -662,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>13.55676328502415</v>
       </c>
@@ -673,7 +674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13.361581920903948</v>
       </c>
@@ -684,7 +685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>10.648148148148152</v>
       </c>
@@ -695,7 +696,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>8.6416861826697993</v>
       </c>
@@ -706,7 +707,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>8.5296684118673713</v>
       </c>
@@ -717,7 +718,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>7.5028248587570623</v>
       </c>
@@ -737,23 +738,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:W35"/>
+    <sheetView topLeftCell="A130" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113:E149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="3"/>
-    <col min="22" max="22" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7265625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.1796875" style="3"/>
+    <col min="22" max="22" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -811,7 +812,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>17.532971295577966</v>
       </c>
@@ -867,7 +868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>22.117541498429787</v>
       </c>
@@ -923,7 +924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>18.156424581005581</v>
       </c>
@@ -979,7 +980,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>11.108490566037737</v>
       </c>
@@ -1020,7 +1021,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>13.581599123767793</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>13.809523809523814</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7.2747014115092172</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>7.7738515901060161</v>
       </c>
@@ -1228,7 +1229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>15.109235495076504</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>16.158357771261002</v>
       </c>
@@ -1320,7 +1321,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>16.158357771261002</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>13.55676328502415</v>
       </c>
@@ -1426,7 +1427,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13.361581920903948</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>10.648148148148152</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>8.6416861826697993</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>8.5296684118673713</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>7.5028248587570623</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>21.26</v>
       </c>
@@ -1698,7 +1699,7 @@
       </c>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A20" s="6">
         <v>17.36</v>
       </c>
@@ -1736,7 +1737,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A21" s="6">
         <v>26.37</v>
       </c>
@@ -1774,7 +1775,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="6">
         <v>37.69</v>
       </c>
@@ -1812,7 +1813,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A23" s="6">
         <v>23.67</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A24" s="6">
         <v>27.15</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A25" s="6">
         <v>42.7</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A26" s="6">
         <v>39.15</v>
       </c>
@@ -1964,7 +1965,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A27" s="6">
         <v>29.57</v>
       </c>
@@ -2002,7 +2003,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A28" s="6">
         <v>28.59</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A29" s="6">
         <v>28.59</v>
       </c>
@@ -2078,7 +2079,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A30" s="6">
         <v>28.63</v>
       </c>
@@ -2116,7 +2117,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="6">
         <v>30.67</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A32" s="6">
         <v>21.23</v>
       </c>
@@ -2192,7 +2193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="6">
         <v>39.01</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A34" s="6">
         <v>41.93</v>
       </c>
@@ -2268,7 +2269,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A35" s="6">
         <v>40.93</v>
       </c>
@@ -2306,7 +2307,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>15</v>
       </c>
@@ -2320,7 +2321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>382.41</v>
       </c>
@@ -2338,7 +2339,7 @@
       </c>
       <c r="T37" s="3"/>
     </row>
-    <row r="38" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>307.25</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>397.04</v>
       </c>
@@ -2373,7 +2374,7 @@
       </c>
       <c r="T39"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>379.77</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>398.56</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>309.10000000000002</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>382.64</v>
       </c>
@@ -2442,7 +2443,7 @@
       </c>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>371.94</v>
       </c>
@@ -2460,7 +2461,7 @@
       </c>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>358</v>
       </c>
@@ -2478,7 +2479,7 @@
       </c>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>382.41</v>
       </c>
@@ -2496,7 +2497,7 @@
       </c>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>385.79</v>
       </c>
@@ -2514,7 +2515,7 @@
       </c>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>500.44</v>
       </c>
@@ -2532,7 +2533,7 @@
       </c>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>385.79</v>
       </c>
@@ -2550,7 +2551,7 @@
       </c>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>377.92200000000003</v>
       </c>
@@ -2568,7 +2569,7 @@
       </c>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>401.11</v>
       </c>
@@ -2586,7 +2587,7 @@
       </c>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>224.69</v>
       </c>
@@ -2604,7 +2605,7 @@
       </c>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>388.88</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>358</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>516.24</v>
       </c>
@@ -2655,7 +2656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>63.78</v>
       </c>
@@ -2673,7 +2674,7 @@
       </c>
       <c r="T56" s="3"/>
     </row>
-    <row r="57" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>358</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>122.28</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>75.489999999999995</v>
       </c>
@@ -2724,7 +2725,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="60" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>264.63</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>105.32</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="62" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>288.45</v>
       </c>
@@ -2775,7 +2776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>81.52</v>
       </c>
@@ -2792,7 +2793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="64" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>144.69999999999999</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>121.38</v>
       </c>
@@ -2826,7 +2827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="66" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>102.56</v>
       </c>
@@ -2843,7 +2844,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>64.11</v>
       </c>
@@ -2860,7 +2861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="68" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>104.87</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>39.229999999999997</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>143.86000000000001</v>
       </c>
@@ -2911,7 +2912,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>65.5</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>24.75</v>
       </c>
@@ -2945,9 +2946,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>15</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>392.97</v>
       </c>
@@ -2978,7 +2979,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>353.24</v>
       </c>
@@ -2996,7 +2997,7 @@
       </c>
       <c r="T77"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>459.56</v>
       </c>
@@ -3015,7 +3016,7 @@
       <c r="H78" s="3"/>
       <c r="T78" s="3"/>
     </row>
-    <row r="79" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>436.45</v>
       </c>
@@ -3033,7 +3034,7 @@
       </c>
       <c r="T79"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>462.18</v>
       </c>
@@ -3051,7 +3052,7 @@
       </c>
       <c r="H80" s="3"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>327.74</v>
       </c>
@@ -3069,7 +3070,7 @@
       </c>
       <c r="H81" s="3"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>419.6</v>
       </c>
@@ -3087,7 +3088,7 @@
       </c>
       <c r="H82" s="3"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>396.05</v>
       </c>
@@ -3105,7 +3106,7 @@
       </c>
       <c r="H83" s="3"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>379.79</v>
       </c>
@@ -3123,7 +3124,7 @@
       </c>
       <c r="H84" s="3"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>392.97</v>
       </c>
@@ -3140,7 +3141,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>422.96</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>436.15</v>
       </c>
@@ -3174,7 +3175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>422.96</v>
       </c>
@@ -3191,7 +3192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="7">
         <v>427.09</v>
       </c>
@@ -3208,7 +3209,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="7">
         <v>465.6</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="7">
         <v>210.18</v>
       </c>
@@ -3242,7 +3243,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>431.2</v>
       </c>
@@ -3259,7 +3260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>379.79</v>
       </c>
@@ -3276,7 +3277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>497.39</v>
       </c>
@@ -3293,7 +3294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>78.180000000000007</v>
       </c>
@@ -3310,7 +3311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>379.79</v>
       </c>
@@ -3327,7 +3328,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>111.35</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>72.89</v>
       </c>
@@ -3361,7 +3362,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>259.51</v>
       </c>
@@ -3378,7 +3379,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>112.61</v>
       </c>
@@ -3395,7 +3396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>315.12</v>
       </c>
@@ -3412,7 +3413,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>100.3</v>
       </c>
@@ -3429,7 +3430,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>142.44</v>
       </c>
@@ -3446,7 +3447,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>118.66</v>
       </c>
@@ -3463,7 +3464,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>95.14</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>69.61</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>110.9</v>
       </c>
@@ -3514,7 +3515,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>45.61</v>
       </c>
@@ -3531,7 +3532,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>154.59</v>
       </c>
@@ -3548,7 +3549,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>79.13</v>
       </c>
@@ -3565,7 +3566,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>31.98</v>
       </c>
@@ -3582,14 +3583,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A112" s="3"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
       <c r="T112" s="3"/>
     </row>
-    <row r="113" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -3607,7 +3608,7 @@
       </c>
       <c r="T113"/>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>0.71</v>
       </c>
@@ -3624,7 +3625,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>0.66</v>
       </c>
@@ -3641,7 +3642,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>0.9</v>
       </c>
@@ -3658,7 +3659,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>0.56000000000000005</v>
       </c>
@@ -3675,7 +3676,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>0.65</v>
       </c>
@@ -3692,7 +3693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>0.8</v>
       </c>
@@ -3709,7 +3710,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>0.64</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>0.98</v>
       </c>
@@ -3743,7 +3744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>1.1599999999999999</v>
       </c>
@@ -3760,7 +3761,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>0.65</v>
       </c>
@@ -3777,7 +3778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>0.7</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>0.7</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A126" s="7">
         <v>0.69</v>
       </c>
@@ -3828,7 +3829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A127" s="7">
         <v>0.73</v>
       </c>
@@ -3845,7 +3846,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A128" s="7">
         <v>0.51</v>
       </c>
@@ -3862,7 +3863,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>1.01</v>
       </c>
@@ -3879,7 +3880,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>1.05</v>
       </c>
@@ -3896,7 +3897,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>1.28</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>1.05</v>
       </c>
@@ -3930,7 +3931,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>0</v>
       </c>
@@ -3947,7 +3948,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>0.23</v>
       </c>
@@ -3964,7 +3965,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>0.24</v>
       </c>
@@ -3981,7 +3982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>0.1</v>
       </c>
@@ -3998,7 +3999,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>0.69</v>
       </c>
@@ -4015,7 +4016,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>0.21</v>
       </c>
@@ -4032,7 +4033,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>0.41</v>
       </c>
@@ -4049,7 +4050,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>0.12</v>
       </c>
@@ -4066,7 +4067,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>0.4</v>
       </c>
@@ -4083,7 +4084,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>0.3</v>
       </c>
@@ -4100,7 +4101,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>0.2</v>
       </c>
@@ -4117,7 +4118,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>0.03</v>
       </c>
@@ -4134,7 +4135,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>0.04</v>
       </c>
@@ -4151,7 +4152,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>0.03</v>
       </c>
@@ -4168,7 +4169,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4185,7 +4186,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>0.15</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>0.04</v>
       </c>
@@ -4226,6 +4227,650 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623FC1DB-9F2D-44D1-9AB7-D341A0292F6F}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>0.71</v>
+      </c>
+      <c r="B2" s="3">
+        <v>400</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>0.66</v>
+      </c>
+      <c r="B3" s="3">
+        <v>400</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>280</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="B5" s="3">
+        <v>280</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="B6" s="3">
+        <v>280</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="B7" s="3">
+        <v>180</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>0.64</v>
+      </c>
+      <c r="B8" s="3">
+        <v>180</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="B9" s="3">
+        <v>180</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="B10" s="3">
+        <v>180</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="B11" s="3">
+        <v>400</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="B12" s="3">
+        <v>400</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>400</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="B14" s="3">
+        <v>280</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="7">
+        <v>0.73</v>
+      </c>
+      <c r="B15" s="3">
+        <v>280</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="7">
+        <v>0.51</v>
+      </c>
+      <c r="B16" s="3">
+        <v>280</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="B17" s="3">
+        <v>180</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="B18" s="3">
+        <v>180</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="B19" s="3">
+        <v>180</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>1.05</v>
+      </c>
+      <c r="B20" s="3">
+        <v>180</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>0</v>
+      </c>
+      <c r="B21" s="3">
+        <v>180</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="B22" s="3">
+        <v>180</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="B23" s="3">
+        <v>180</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B24" s="3">
+        <v>180</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>0.69</v>
+      </c>
+      <c r="B25" s="3">
+        <v>240</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="B26" s="3">
+        <v>240</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="B27" s="3">
+        <v>240</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="B28" s="3">
+        <v>240</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="B29" s="3">
+        <v>240</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="B30" s="3">
+        <v>300</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="B31" s="3">
+        <v>300</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="B32" s="3">
+        <v>300</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="B33" s="3">
+        <v>300</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="B34" s="3">
+        <v>300</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="B35" s="3">
+        <v>400</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="B36" s="3">
+        <v>400</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="B37" s="3">
+        <v>400</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR45"/>
   <sheetViews>
@@ -4233,29 +4878,29 @@
       <selection activeCell="K8" sqref="K8:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="8" max="8" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" style="3" customWidth="1"/>
     <col min="12" max="12" width="7" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.85546875" style="3" customWidth="1"/>
-    <col min="27" max="27" width="9.7109375" style="3" customWidth="1"/>
+    <col min="13" max="13" width="7.81640625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.1796875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="18.26953125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1796875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.81640625" style="3" customWidth="1"/>
+    <col min="27" max="27" width="9.7265625" style="3" customWidth="1"/>
     <col min="28" max="29" width="11" style="3" customWidth="1"/>
-    <col min="31" max="34" width="9.140625" style="3"/>
-    <col min="38" max="38" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="9.1796875" style="3"/>
+    <col min="38" max="38" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4375,7 +5020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>400</v>
       </c>
@@ -4498,7 +5143,7 @@
         <v>0.71</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>300</v>
       </c>
@@ -4621,7 +5266,7 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>200</v>
       </c>
@@ -4721,7 +5366,7 @@
       <c r="AK4" s="3"/>
       <c r="AL4" s="3"/>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>100</v>
       </c>
@@ -4794,7 +5439,7 @@
       </c>
       <c r="AJ5" s="3"/>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>50</v>
       </c>
@@ -4842,7 +5487,7 @@
       </c>
       <c r="AJ6" s="3"/>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>400</v>
       </c>
@@ -4891,7 +5536,7 @@
       </c>
       <c r="AJ7" s="3"/>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>500</v>
       </c>
@@ -4939,7 +5584,7 @@
       </c>
       <c r="AJ8" s="3"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>600</v>
       </c>
@@ -4987,7 +5632,7 @@
       </c>
       <c r="AJ9" s="3"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>700</v>
       </c>
@@ -5035,7 +5680,7 @@
       </c>
       <c r="AJ10" s="3"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>800</v>
       </c>
@@ -5083,7 +5728,7 @@
       </c>
       <c r="AJ11" s="3"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>900</v>
       </c>
@@ -5131,7 +5776,7 @@
       </c>
       <c r="AJ12" s="3"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>400</v>
       </c>
@@ -5179,7 +5824,7 @@
       </c>
       <c r="AJ13" s="3"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>300</v>
       </c>
@@ -5226,7 +5871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>200</v>
       </c>
@@ -5273,7 +5918,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>100</v>
       </c>
@@ -5320,7 +5965,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>50</v>
       </c>
@@ -5367,7 +6012,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>400</v>
       </c>
@@ -5414,7 +6059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>500</v>
       </c>
@@ -5461,7 +6106,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>600</v>
       </c>
@@ -5508,7 +6153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>700</v>
       </c>
@@ -5555,7 +6200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>800</v>
       </c>
@@ -5602,7 +6247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>900</v>
       </c>
@@ -5649,7 +6294,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>400</v>
       </c>
@@ -5681,7 +6326,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>300</v>
       </c>
@@ -5713,7 +6358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>200</v>
       </c>
@@ -5745,7 +6390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>100</v>
       </c>
@@ -5777,7 +6422,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>50</v>
       </c>
@@ -5809,7 +6454,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>400</v>
       </c>
@@ -5841,7 +6486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>500</v>
       </c>
@@ -5873,7 +6518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>600</v>
       </c>
@@ -5905,7 +6550,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>700</v>
       </c>
@@ -5937,7 +6582,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>800</v>
       </c>
@@ -5969,7 +6614,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>900</v>
       </c>
@@ -6001,7 +6646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>400</v>
       </c>
@@ -6018,7 +6663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>300</v>
       </c>
@@ -6035,7 +6680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>200</v>
       </c>
@@ -6052,7 +6697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>100</v>
       </c>
@@ -6069,7 +6714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>50</v>
       </c>
@@ -6086,7 +6731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>400</v>
       </c>
@@ -6103,7 +6748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>500</v>
       </c>
@@ -6120,7 +6765,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>600</v>
       </c>
@@ -6137,7 +6782,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>700</v>
       </c>
@@ -6154,7 +6799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>800</v>
       </c>
@@ -6171,7 +6816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>900</v>
       </c>
@@ -6193,7 +6838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AR45"/>
   <sheetViews>
@@ -6201,27 +6846,27 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="3"/>
+    <col min="1" max="5" width="9.1796875" style="3"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="11" style="3" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="15" width="18.28515625" style="3" customWidth="1"/>
-    <col min="16" max="20" width="9.140625" style="3"/>
-    <col min="23" max="23" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.140625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.28515625" style="3" customWidth="1"/>
-    <col min="27" max="29" width="18.28515625" style="8" customWidth="1"/>
-    <col min="30" max="30" width="11.140625" style="3" customWidth="1"/>
-    <col min="31" max="34" width="9.140625" style="3"/>
-    <col min="38" max="38" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="18.26953125" style="3" customWidth="1"/>
+    <col min="16" max="20" width="9.1796875" style="3"/>
+    <col min="23" max="23" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.1796875" style="3" customWidth="1"/>
+    <col min="25" max="25" width="18.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.26953125" style="3" customWidth="1"/>
+    <col min="27" max="29" width="18.26953125" style="8" customWidth="1"/>
+    <col min="30" max="30" width="11.1796875" style="3" customWidth="1"/>
+    <col min="31" max="34" width="9.1796875" style="3"/>
+    <col min="38" max="38" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6340,7 +6985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>400</v>
       </c>
@@ -6462,7 +7107,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>300</v>
       </c>
@@ -6584,7 +7229,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>200</v>
       </c>
@@ -6706,7 +7351,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>100</v>
       </c>
@@ -6781,7 +7426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>50</v>
       </c>
@@ -6828,7 +7473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>400</v>
       </c>
@@ -6878,7 +7523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>500</v>
       </c>
@@ -6938,7 +7583,7 @@
       <c r="AM8" s="6"/>
       <c r="AN8" s="6"/>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>600</v>
       </c>
@@ -6996,7 +7641,7 @@
       <c r="AM9" s="6"/>
       <c r="AN9" s="6"/>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>700</v>
       </c>
@@ -7055,7 +7700,7 @@
       <c r="AM10" s="6"/>
       <c r="AN10" s="6"/>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>800</v>
       </c>
@@ -7114,7 +7759,7 @@
       <c r="AM11" s="6"/>
       <c r="AN11" s="6"/>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>900</v>
       </c>
@@ -7173,7 +7818,7 @@
       <c r="AM12" s="6"/>
       <c r="AN12" s="6"/>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>400</v>
       </c>
@@ -7232,7 +7877,7 @@
       <c r="AM13" s="6"/>
       <c r="AN13" s="6"/>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>300</v>
       </c>
@@ -7288,7 +7933,7 @@
       <c r="AM14" s="6"/>
       <c r="AN14" s="6"/>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>200</v>
       </c>
@@ -7344,7 +7989,7 @@
       <c r="AM15" s="6"/>
       <c r="AN15" s="6"/>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>100</v>
       </c>
@@ -7400,7 +8045,7 @@
       <c r="AM16" s="6"/>
       <c r="AN16" s="6"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>50</v>
       </c>
@@ -7456,7 +8101,7 @@
       <c r="AM17" s="6"/>
       <c r="AN17" s="6"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>400</v>
       </c>
@@ -7509,7 +8154,7 @@
       <c r="AM18" s="6"/>
       <c r="AN18" s="6"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>500</v>
       </c>
@@ -7556,7 +8201,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>600</v>
       </c>
@@ -7603,7 +8248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>700</v>
       </c>
@@ -7650,7 +8295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>800</v>
       </c>
@@ -7697,7 +8342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>900</v>
       </c>
@@ -7744,7 +8389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>400</v>
       </c>
@@ -7791,7 +8436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>300</v>
       </c>
@@ -7838,7 +8483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>200</v>
       </c>
@@ -7885,7 +8530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>100</v>
       </c>
@@ -7932,7 +8577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>50</v>
       </c>
@@ -7979,7 +8624,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>400</v>
       </c>
@@ -8026,7 +8671,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>500</v>
       </c>
@@ -8073,7 +8718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>600</v>
       </c>
@@ -8120,7 +8765,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>700</v>
       </c>
@@ -8167,7 +8812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>800</v>
       </c>
@@ -8214,7 +8859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>900</v>
       </c>
@@ -8261,7 +8906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>400</v>
       </c>
@@ -8280,7 +8925,7 @@
       <c r="S35" s="4"/>
       <c r="AH35" s="4"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>300</v>
       </c>
@@ -8299,7 +8944,7 @@
       <c r="S36" s="4"/>
       <c r="AH36" s="4"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>200</v>
       </c>
@@ -8318,7 +8963,7 @@
       <c r="S37" s="4"/>
       <c r="AH37" s="4"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>100</v>
       </c>
@@ -8337,7 +8982,7 @@
       <c r="S38" s="4"/>
       <c r="AH38" s="4"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>50</v>
       </c>
@@ -8356,7 +9001,7 @@
       <c r="S39" s="4"/>
       <c r="AH39" s="4"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>400</v>
       </c>
@@ -8375,7 +9020,7 @@
       <c r="S40" s="4"/>
       <c r="AH40" s="4"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>500</v>
       </c>
@@ -8394,7 +9039,7 @@
       <c r="S41" s="4"/>
       <c r="AH41" s="4"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>600</v>
       </c>
@@ -8413,7 +9058,7 @@
       <c r="S42" s="4"/>
       <c r="AH42" s="4"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>700</v>
       </c>
@@ -8432,7 +9077,7 @@
       <c r="S43" s="4"/>
       <c r="AH43" s="4"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>800</v>
       </c>
@@ -8451,7 +9096,7 @@
       <c r="S44" s="4"/>
       <c r="AH44" s="4"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>900</v>
       </c>
@@ -8476,7 +9121,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7157326-4056-4411-B4A6-C12E6047962B}">
   <dimension ref="A1:H111"/>
   <sheetViews>
@@ -8484,13 +9129,13 @@
       <selection activeCell="A111" sqref="A1:E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.1796875" style="3"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -8507,7 +9152,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>50</v>
       </c>
@@ -8525,7 +9170,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>100</v>
       </c>
@@ -8543,7 +9188,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>200</v>
       </c>
@@ -8561,7 +9206,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>300</v>
       </c>
@@ -8579,7 +9224,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>400</v>
       </c>
@@ -8597,7 +9242,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>500</v>
       </c>
@@ -8615,7 +9260,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>600</v>
       </c>
@@ -8633,7 +9278,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>700</v>
       </c>
@@ -8651,7 +9296,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>800</v>
       </c>
@@ -8669,7 +9314,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>900</v>
       </c>
@@ -8687,7 +9332,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>1000</v>
       </c>
@@ -8705,7 +9350,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>50</v>
       </c>
@@ -8723,7 +9368,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>100</v>
       </c>
@@ -8741,7 +9386,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>200</v>
       </c>
@@ -8759,7 +9404,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>300</v>
       </c>
@@ -8777,7 +9422,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>400</v>
       </c>
@@ -8795,7 +9440,7 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>500</v>
       </c>
@@ -8813,7 +9458,7 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>600</v>
       </c>
@@ -8831,7 +9476,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>700</v>
       </c>
@@ -8849,7 +9494,7 @@
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>800</v>
       </c>
@@ -8867,7 +9512,7 @@
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>900</v>
       </c>
@@ -8885,7 +9530,7 @@
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>1000</v>
       </c>
@@ -8903,7 +9548,7 @@
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>50</v>
       </c>
@@ -8921,7 +9566,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>100</v>
       </c>
@@ -8939,7 +9584,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>200</v>
       </c>
@@ -8957,7 +9602,7 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>300</v>
       </c>
@@ -8975,7 +9620,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>400</v>
       </c>
@@ -8993,7 +9638,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>500</v>
       </c>
@@ -9011,7 +9656,7 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>600</v>
       </c>
@@ -9029,7 +9674,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>700</v>
       </c>
@@ -9047,7 +9692,7 @@
       </c>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>800</v>
       </c>
@@ -9065,7 +9710,7 @@
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>900</v>
       </c>
@@ -9083,7 +9728,7 @@
       </c>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>1000</v>
       </c>
@@ -9101,7 +9746,7 @@
       </c>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>50</v>
       </c>
@@ -9118,7 +9763,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>100</v>
       </c>
@@ -9135,7 +9780,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>200</v>
       </c>
@@ -9152,7 +9797,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>300</v>
       </c>
@@ -9169,7 +9814,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>400</v>
       </c>
@@ -9186,7 +9831,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>500</v>
       </c>
@@ -9203,7 +9848,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>600</v>
       </c>
@@ -9220,7 +9865,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>700</v>
       </c>
@@ -9237,7 +9882,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>800</v>
       </c>
@@ -9254,7 +9899,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>900</v>
       </c>
@@ -9271,7 +9916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>1000</v>
       </c>
@@ -9288,7 +9933,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>50</v>
       </c>
@@ -9305,7 +9950,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>100</v>
       </c>
@@ -9323,7 +9968,7 @@
       </c>
       <c r="H47" s="6"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>200</v>
       </c>
@@ -9341,7 +9986,7 @@
       </c>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>300</v>
       </c>
@@ -9359,7 +10004,7 @@
       </c>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>400</v>
       </c>
@@ -9378,7 +10023,7 @@
       <c r="F50" s="6"/>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>500</v>
       </c>
@@ -9397,7 +10042,7 @@
       <c r="F51" s="6"/>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>600</v>
       </c>
@@ -9416,7 +10061,7 @@
       <c r="F52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>700</v>
       </c>
@@ -9435,7 +10080,7 @@
       <c r="F53" s="6"/>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>800</v>
       </c>
@@ -9454,7 +10099,7 @@
       <c r="F54" s="6"/>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>900</v>
       </c>
@@ -9473,7 +10118,7 @@
       <c r="F55" s="6"/>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>1000</v>
       </c>
@@ -9492,7 +10137,7 @@
       <c r="F56" s="6"/>
       <c r="H56" s="6"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>50</v>
       </c>
@@ -9511,7 +10156,7 @@
       <c r="F57" s="6"/>
       <c r="H57" s="6"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>100</v>
       </c>
@@ -9529,7 +10174,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>200</v>
       </c>
@@ -9547,7 +10192,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>300</v>
       </c>
@@ -9565,7 +10210,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>400</v>
       </c>
@@ -9582,7 +10227,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>500</v>
       </c>
@@ -9599,7 +10244,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>600</v>
       </c>
@@ -9616,7 +10261,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>700</v>
       </c>
@@ -9633,7 +10278,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>800</v>
       </c>
@@ -9650,7 +10295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>900</v>
       </c>
@@ -9667,7 +10312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>1000</v>
       </c>
@@ -9684,7 +10329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>50</v>
       </c>
@@ -9701,7 +10346,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>100</v>
       </c>
@@ -9718,7 +10363,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>200</v>
       </c>
@@ -9735,7 +10380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>300</v>
       </c>
@@ -9752,7 +10397,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>400</v>
       </c>
@@ -9769,7 +10414,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>500</v>
       </c>
@@ -9786,7 +10431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>600</v>
       </c>
@@ -9803,7 +10448,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>700</v>
       </c>
@@ -9820,7 +10465,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>800</v>
       </c>
@@ -9837,7 +10482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>900</v>
       </c>
@@ -9854,7 +10499,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>1000</v>
       </c>
@@ -9871,7 +10516,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>50</v>
       </c>
@@ -9888,7 +10533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>100</v>
       </c>
@@ -9905,7 +10550,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>200</v>
       </c>
@@ -9922,7 +10567,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>300</v>
       </c>
@@ -9939,7 +10584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>400</v>
       </c>
@@ -9956,7 +10601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>500</v>
       </c>
@@ -9973,7 +10618,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>600</v>
       </c>
@@ -9990,7 +10635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>700</v>
       </c>
@@ -10007,7 +10652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>800</v>
       </c>
@@ -10024,7 +10669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>900</v>
       </c>
@@ -10041,7 +10686,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>1000</v>
       </c>
@@ -10058,7 +10703,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>50</v>
       </c>
@@ -10075,7 +10720,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>100</v>
       </c>
@@ -10092,7 +10737,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>200</v>
       </c>
@@ -10109,7 +10754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>300</v>
       </c>
@@ -10126,7 +10771,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>400</v>
       </c>
@@ -10143,7 +10788,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>500</v>
       </c>
@@ -10160,7 +10805,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>600</v>
       </c>
@@ -10177,7 +10822,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>700</v>
       </c>
@@ -10194,7 +10839,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>800</v>
       </c>
@@ -10211,7 +10856,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>900</v>
       </c>
@@ -10228,7 +10873,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>1000</v>
       </c>
@@ -10245,7 +10890,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>50</v>
       </c>
@@ -10262,7 +10907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>100</v>
       </c>
@@ -10279,7 +10924,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>200</v>
       </c>
@@ -10296,7 +10941,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>300</v>
       </c>
@@ -10313,7 +10958,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>400</v>
       </c>
@@ -10330,7 +10975,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>500</v>
       </c>
@@ -10347,7 +10992,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>600</v>
       </c>
@@ -10364,7 +11009,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>700</v>
       </c>
@@ -10381,7 +11026,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>800</v>
       </c>
@@ -10398,7 +11043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>900</v>
       </c>
@@ -10415,7 +11060,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>1000</v>
       </c>

</xml_diff>